<commit_message>
working on improving captions! IP
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -1,35 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217749D1-9110-420F-A469-458217469716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC937812-1299-4C6D-894F-DAC3C249E4F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YS" sheetId="1" r:id="rId1"/>
     <sheet name="SW" sheetId="2" r:id="rId2"/>
     <sheet name="YI" sheetId="3" r:id="rId3"/>
-    <sheet name="YN" sheetId="4" r:id="rId4"/>
-    <sheet name="6MC" sheetId="5" r:id="rId5"/>
-    <sheet name="DC" sheetId="6" r:id="rId6"/>
-    <sheet name="PBMS" sheetId="7" r:id="rId7"/>
-    <sheet name="PBSF" sheetId="8" r:id="rId8"/>
-    <sheet name="ME" sheetId="10" r:id="rId9"/>
-    <sheet name="MO" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId4"/>
+    <sheet name="YN" sheetId="4" r:id="rId5"/>
+    <sheet name="6MC" sheetId="5" r:id="rId6"/>
+    <sheet name="DC" sheetId="6" r:id="rId7"/>
+    <sheet name="PBMS" sheetId="7" r:id="rId8"/>
+    <sheet name="PBSF" sheetId="8" r:id="rId9"/>
+    <sheet name="ME" sheetId="10" r:id="rId10"/>
+    <sheet name="MO" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
   <si>
     <t>chloride_mgL</t>
   </si>
@@ -47,6 +48,12 @@
   </si>
   <si>
     <t>Depth_m</t>
+  </si>
+  <si>
+    <t>I changed dates in the YI datetime collected. During a portion of the record, discharge data was only collected 4 times a day. I can't figure out how to left_join by closest time so changing at this point. Actual datetime is in column, actual_datetime</t>
+  </si>
+  <si>
+    <t>actual_datetime</t>
   </si>
 </sst>
 </file>
@@ -535,12 +542,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -902,16 +913,16 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -925,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.505555555559</v>
       </c>
@@ -939,7 +950,7 @@
         <v>64.31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.506249999999</v>
       </c>
@@ -953,7 +964,7 @@
         <v>64.739999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.397222222222</v>
       </c>
@@ -967,7 +978,7 @@
         <v>64.95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.566666666666</v>
       </c>
@@ -981,7 +992,7 @@
         <v>65.571906466400335</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.577777777777</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>65.593052538044802</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.575694444444</v>
       </c>
@@ -1009,7 +1020,7 @@
         <v>65.661689578674412</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.575694444444</v>
       </c>
@@ -1020,7 +1031,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.573611111111</v>
       </c>
@@ -1031,7 +1042,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.580555555556</v>
       </c>
@@ -1042,7 +1053,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.572222222225</v>
       </c>
@@ -1050,7 +1061,7 @@
         <v>43888.572222222225</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.574999999997</v>
       </c>
@@ -1058,12 +1069,12 @@
         <v>43895.575694444444</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.529861111114</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43906.356249999997</v>
       </c>
@@ -1075,6 +1086,112 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3A990-AAD2-449A-8315-183C290E8A9C}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43888.587500000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43888.586805555555</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43888.588888888888</v>
+      </c>
+      <c r="D4" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43888.59097222222</v>
+      </c>
+      <c r="D5" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43888.59097222222</v>
+      </c>
+      <c r="D6" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43888.593055555553</v>
+      </c>
+      <c r="D7" s="2">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D91DE40-05E6-4B37-9CD8-EC471F027E06}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1082,16 +1199,16 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1108,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43888.5</v>
       </c>
@@ -1119,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43888.5</v>
       </c>
@@ -1130,7 +1247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43888.5</v>
       </c>
@@ -1141,7 +1258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43888.5</v>
       </c>
@@ -1152,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43888.5</v>
       </c>
@@ -1163,7 +1280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43889.5</v>
       </c>
@@ -1187,16 +1304,16 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.477083333331</v>
       </c>
@@ -1224,7 +1341,7 @@
         <v>161.12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.529861111114</v>
       </c>
@@ -1238,7 +1355,7 @@
         <v>145.31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.415277777778</v>
       </c>
@@ -1252,7 +1369,7 @@
         <v>154.22999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.586111111108</v>
       </c>
@@ -1266,7 +1383,7 @@
         <v>429.28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.602777777778</v>
       </c>
@@ -1280,7 +1397,7 @@
         <v>220.37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.595138888886</v>
       </c>
@@ -1294,7 +1411,7 @@
         <v>497.34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.59097222222</v>
       </c>
@@ -1305,7 +1422,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.593055555553</v>
       </c>
@@ -1316,7 +1433,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.600694444445</v>
       </c>
@@ -1327,7 +1444,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.588888888888</v>
       </c>
@@ -1335,7 +1452,7 @@
         <v>43888.567361111112</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.597916666666</v>
       </c>
@@ -1343,12 +1460,12 @@
         <v>43895.580555555556</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.546527777777</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43906.376388888886</v>
       </c>
@@ -1360,175 +1477,217 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.464583333334</v>
       </c>
       <c r="B2" s="1">
+        <v>43816.416666666664</v>
+      </c>
+      <c r="C2" s="1">
         <v>43846.413194444445</v>
       </c>
-      <c r="C2" s="4">
+      <c r="D2" s="4">
         <v>43865</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>52.39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.57708333333</v>
       </c>
       <c r="B3" s="1">
+        <v>43830.666666666664</v>
+      </c>
+      <c r="C3" s="1">
         <v>43846.456250000003</v>
       </c>
-      <c r="C3" s="4">
+      <c r="D3" s="4">
         <v>43865</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>52.01</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.429861111108</v>
       </c>
       <c r="B4" s="1">
+        <v>43836.416666666664</v>
+      </c>
+      <c r="C4" s="1">
         <v>43846.451388888891</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="4">
         <v>43865</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>53.78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.6</v>
       </c>
       <c r="B5" s="1">
+        <v>43844.666666666664</v>
+      </c>
+      <c r="C5" s="1">
         <v>43853.595138888886</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="4">
         <v>43873</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>56.355273063000688</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.618055555555</v>
       </c>
       <c r="B6" s="1">
+        <v>43851.618055555555</v>
+      </c>
+      <c r="C6" s="1">
         <v>43853.61041666667</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="4">
         <v>43873</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>53.341090594049632</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.609027777777</v>
       </c>
       <c r="B7" s="1">
+        <v>43858.609027777777</v>
+      </c>
+      <c r="C7" s="1">
         <v>43836.60833333333</v>
       </c>
-      <c r="C7" s="4">
+      <c r="D7" s="4">
         <v>43873</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>53.634368734344861</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.605555555558</v>
       </c>
       <c r="B8" s="1">
+        <v>43865.605555555558</v>
+      </c>
+      <c r="C8" s="1">
         <v>43874.595138888886</v>
       </c>
-      <c r="C8" s="4">
+      <c r="D8" s="4">
         <v>43892</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.606944444444</v>
       </c>
       <c r="B9" s="1">
+        <v>43872.606944444444</v>
+      </c>
+      <c r="C9" s="1">
         <v>43874.567361111112</v>
       </c>
-      <c r="C9" s="4">
+      <c r="D9" s="4">
         <v>43892</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.616666666669</v>
       </c>
       <c r="B10" s="1">
+        <v>43879.616666666669</v>
+      </c>
+      <c r="C10" s="1">
         <v>43881.576388888891</v>
       </c>
-      <c r="C10" s="4">
+      <c r="D10" s="4">
         <v>43892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.603472222225</v>
       </c>
       <c r="B11" s="1">
+        <v>43886.603472222225</v>
+      </c>
+      <c r="C11" s="1">
         <v>43888.577777777777</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.613888888889</v>
       </c>
       <c r="B12" s="1">
+        <v>43893.613888888889</v>
+      </c>
+      <c r="C12" s="1">
         <v>43895.56527777778</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.060416666667</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>43900.060416666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
+        <v>43906.38958333333</v>
+      </c>
+      <c r="B14" s="1">
         <v>43906.38958333333</v>
       </c>
     </row>
@@ -1538,6 +1697,80 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1ABF87B-2C3E-4ACD-AB93-9661038D3DBF}">
+  <dimension ref="B2:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -1545,16 +1778,16 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1568,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.446527777778</v>
       </c>
@@ -1582,7 +1815,7 @@
         <v>53.197903408657218</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.6</v>
       </c>
@@ -1596,7 +1829,7 @@
         <v>38.01</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.445833333331</v>
       </c>
@@ -1610,7 +1843,7 @@
         <v>49.92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.618055555555</v>
       </c>
@@ -1624,7 +1857,7 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.635416666664</v>
       </c>
@@ -1638,7 +1871,7 @@
         <v>50.652847736295882</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.624305555553</v>
       </c>
@@ -1652,7 +1885,7 @@
         <v>67.436843174760639</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.625</v>
       </c>
@@ -1663,7 +1896,7 @@
         <v>43910</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.621527777781</v>
       </c>
@@ -1674,7 +1907,7 @@
         <v>43910</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.630555555559</v>
       </c>
@@ -1685,7 +1918,7 @@
         <v>43910</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.616666666669</v>
       </c>
@@ -1693,7 +1926,7 @@
         <v>43888.576388888891</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.628472222219</v>
       </c>
@@ -1701,12 +1934,12 @@
         <v>43895.569444444445</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.574305555558</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43906.40625</v>
       </c>
@@ -1716,7 +1949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -1724,16 +1957,16 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1747,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.631249999999</v>
       </c>
@@ -1761,7 +1994,7 @@
         <v>42.99</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.613194444442</v>
       </c>
@@ -1775,7 +2008,7 @@
         <v>37.76</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.461111111108</v>
       </c>
@@ -1789,7 +2022,7 @@
         <v>43.25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.627083333333</v>
       </c>
@@ -1803,7 +2036,7 @@
         <v>45.582503159530503</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.647222222222</v>
       </c>
@@ -1817,7 +2050,7 @@
         <v>46.216873912486122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.634027777778</v>
       </c>
@@ -1831,7 +2064,7 @@
         <v>47.815486925581425</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.640972222223</v>
       </c>
@@ -1842,7 +2075,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.629861111112</v>
       </c>
@@ -1853,7 +2086,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.640277777777</v>
       </c>
@@ -1864,7 +2097,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.625</v>
       </c>
@@ -1872,7 +2105,7 @@
         <v>43888.584027777775</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.638888888891</v>
       </c>
@@ -1880,12 +2113,12 @@
         <v>43895.585416666669</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.582638888889</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43906.416666666664</v>
       </c>
@@ -1895,7 +2128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -1903,16 +2136,16 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1926,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.426388888889</v>
       </c>
@@ -1940,7 +2173,7 @@
         <v>37.340000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.625</v>
       </c>
@@ -1954,7 +2187,7 @@
         <v>42.09</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.468055555553</v>
       </c>
@@ -1968,7 +2201,7 @@
         <v>37.619999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.636805555558</v>
       </c>
@@ -1982,7 +2215,7 @@
         <v>36.153569983537686</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.658333333333</v>
       </c>
@@ -1996,7 +2229,7 @@
         <v>35.844941153177423</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.64166666667</v>
       </c>
@@ -2010,7 +2243,7 @@
         <v>39.674826842412301</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.65347222222</v>
       </c>
@@ -2021,7 +2254,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.634722222225</v>
       </c>
@@ -2032,7 +2265,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.645833333336</v>
       </c>
@@ -2043,7 +2276,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.631249999999</v>
       </c>
@@ -2051,7 +2284,7 @@
         <v>43888.582638888889</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.652777777781</v>
       </c>
@@ -2059,12 +2292,12 @@
         <v>43895.561111111114</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.59097222222</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43906.427083333336</v>
       </c>
@@ -2074,7 +2307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -2082,16 +2315,16 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2105,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.411805555559</v>
       </c>
@@ -2119,7 +2352,7 @@
         <v>110.52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.63958333333</v>
       </c>
@@ -2133,7 +2366,7 @@
         <v>117.82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.480555555558</v>
       </c>
@@ -2147,7 +2380,7 @@
         <v>147.49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.649305555555</v>
       </c>
@@ -2161,7 +2394,7 @@
         <v>131.26073933647763</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.173611111109</v>
       </c>
@@ -2175,7 +2408,7 @@
         <v>124.12080489218306</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.654166666667</v>
       </c>
@@ -2189,7 +2422,7 @@
         <v>168.46246480925123</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.67083333333</v>
       </c>
@@ -2200,7 +2433,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.647222222222</v>
       </c>
@@ -2211,7 +2444,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.659722222219</v>
       </c>
@@ -2222,7 +2455,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.644444444442</v>
       </c>
@@ -2230,7 +2463,7 @@
         <v>43888.568055555559</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.670138888891</v>
       </c>
@@ -2238,12 +2471,12 @@
         <v>43895.585416666669</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.603472222225</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43906.441666666666</v>
       </c>
@@ -2253,23 +2486,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2283,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43816.402777777781</v>
       </c>
@@ -2297,7 +2530,7 @@
         <v>478.98</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43830.649305555555</v>
       </c>
@@ -2311,7 +2544,7 @@
         <v>168.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43836.488888888889</v>
       </c>
@@ -2325,7 +2558,7 @@
         <v>250.14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43844.658333333333</v>
       </c>
@@ -2339,7 +2572,7 @@
         <v>666.1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43851.68472222222</v>
       </c>
@@ -2353,7 +2586,7 @@
         <v>613.4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43858.664583333331</v>
       </c>
@@ -2367,7 +2600,7 @@
         <v>722.91</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43865.676388888889</v>
       </c>
@@ -2378,7 +2611,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43872.652777777781</v>
       </c>
@@ -2389,7 +2622,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43879.666666666664</v>
       </c>
@@ -2400,7 +2633,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43886.65</v>
       </c>
@@ -2408,7 +2641,7 @@
         <v>43888.572916666664</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43893.677777777775</v>
       </c>
@@ -2416,12 +2649,12 @@
         <v>43895.598611111112</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43900.612500000003</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43906.451388888891</v>
       </c>
@@ -2430,110 +2663,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3A990-AAD2-449A-8315-183C290E8A9C}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43888.587500000001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43888.586805555555</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43888.588888888888</v>
-      </c>
-      <c r="D4" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43888.59097222222</v>
-      </c>
-      <c r="D5" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43888.59097222222</v>
-      </c>
-      <c r="D6" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43888.593055555553</v>
-      </c>
-      <c r="D7" s="2">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
some figures for presentations
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF64D8A-B6CB-46B4-BBCA-DD2284D7437D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A777F1-FFF5-4580-ADB6-ABB07E476793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -938,7 +938,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,6 +1303,9 @@
       <c r="D22" s="4">
         <v>44203</v>
       </c>
+      <c r="E22" s="2">
+        <v>149.20769117935939</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1316,6 +1319,9 @@
       </c>
       <c r="D23" s="4">
         <v>44203</v>
+      </c>
+      <c r="E23" s="2">
+        <v>135.29934855581524</v>
       </c>
     </row>
   </sheetData>
@@ -1327,7 +1333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3A990-AAD2-449A-8315-183C290E8A9C}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -2231,8 +2237,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35:D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2772,6 +2778,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>63.398039954705133</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -2785,6 +2794,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>63.593059984680025</v>
       </c>
     </row>
   </sheetData>
@@ -2797,9 +2809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3342,6 +3354,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>185.04099537562053</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -3355,6 +3370,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>173.52262605634044</v>
       </c>
     </row>
   </sheetData>
@@ -3367,8 +3385,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35:D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3912,6 +3930,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>50.228920294925295</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -3925,6 +3946,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>51.894840328009309</v>
       </c>
     </row>
   </sheetData>
@@ -3937,8 +3961,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35:D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4481,6 +4505,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>47.043545551602335</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -4494,6 +4521,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>42.887212448968732</v>
       </c>
     </row>
   </sheetData>
@@ -4507,8 +4537,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35:D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5051,6 +5081,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>42.507227959174934</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -5064,6 +5097,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>41.731867766926307</v>
       </c>
     </row>
   </sheetData>
@@ -5076,8 +5112,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35:D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5620,6 +5656,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>31.839202892037115</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -5633,6 +5672,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>32.255734819969838</v>
       </c>
     </row>
   </sheetData>
@@ -5645,8 +5687,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35:D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6189,6 +6231,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>115.26559144657953</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -6202,6 +6247,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>119.63477651641556</v>
       </c>
     </row>
   </sheetData>
@@ -6213,9 +6261,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6761,6 +6809,9 @@
       <c r="D35" s="4">
         <v>44203</v>
       </c>
+      <c r="E35" s="2">
+        <v>542.87125689376614</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
@@ -6774,6 +6825,9 @@
       </c>
       <c r="D36" s="4">
         <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>549.01870258922099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on creating tables of watershed characteristics
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2D44AC-64E4-4F82-8A40-A3EFB31B3A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE96F3FC-ACA6-4F41-9C7B-884ACAB14C45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -938,7 +938,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,6 +1336,9 @@
       </c>
       <c r="D24" s="4">
         <v>44210</v>
+      </c>
+      <c r="E24" s="2">
+        <v>139.54591516332971</v>
       </c>
     </row>
   </sheetData>
@@ -2251,8 +2254,8 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2826,6 +2829,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>64.470604910098302</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2839,7 +2845,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3416,6 +3422,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>155.29272259448322</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3428,7 +3437,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4006,6 +4015,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>53.197881809201277</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4018,7 +4030,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4595,6 +4607,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>46.519491182570441</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4608,7 +4623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5185,6 +5200,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>42.88645793827957</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5197,7 +5215,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5774,6 +5792,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>32.771157813637501</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5786,7 +5807,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6363,6 +6384,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>105.46460615166298</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6375,7 +6399,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6955,6 +6979,9 @@
       <c r="D37" s="4">
         <v>44210</v>
       </c>
+      <c r="E37" s="2">
+        <v>538.61968893977576</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on QC plots now. tricky visualization to figure out next (inspo from Knapp et al., 2020)
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39483ABE-E8F9-4E7F-A8D8-1DE8B28FB7AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BB2D45-BE04-4CB6-8F38-6407CA26C05B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -938,7 +938,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D25" sqref="D25:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1351,6 +1351,12 @@
       <c r="C25" s="1">
         <v>44215.444444444445</v>
       </c>
+      <c r="D25" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E25" s="2">
+        <v>152.64632975884538</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1362,6 +1368,12 @@
       <c r="C26" s="1">
         <v>44222.418055555558</v>
       </c>
+      <c r="D26" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E26" s="2">
+        <v>145.78513134791959</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1372,6 +1384,12 @@
       </c>
       <c r="C27" s="1">
         <v>44229.390277777777</v>
+      </c>
+      <c r="D27" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E27" s="2">
+        <v>153.57946686317692</v>
       </c>
     </row>
   </sheetData>
@@ -1875,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D91DE40-05E6-4B37-9CD8-EC471F027E06}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2287,6 +2305,9 @@
       <c r="D26" s="2">
         <v>0</v>
       </c>
+      <c r="E26" s="2">
+        <v>62.793626483308309</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -2298,6 +2319,9 @@
       <c r="D27" s="2">
         <v>4</v>
       </c>
+      <c r="E27" s="2">
+        <v>62.736164526843595</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -2309,6 +2333,9 @@
       <c r="D28" s="2">
         <v>8</v>
       </c>
+      <c r="E28" s="2">
+        <v>63.641441065559135</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -2320,6 +2347,9 @@
       <c r="D29" s="2">
         <v>12</v>
       </c>
+      <c r="E29" s="2">
+        <v>65.738746566764036</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -2331,6 +2361,9 @@
       <c r="D30" s="2">
         <v>16</v>
       </c>
+      <c r="E30" s="2">
+        <v>91.144478590790229</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
@@ -2341,6 +2374,9 @@
       </c>
       <c r="D31" s="2">
         <v>20</v>
+      </c>
+      <c r="E31" s="2">
+        <v>121.33676729410395</v>
       </c>
     </row>
   </sheetData>
@@ -2353,8 +2389,8 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A40"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2942,6 +2978,12 @@
       <c r="C38" s="1">
         <v>44215.461805555555</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>63.22087685333323</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -2953,6 +2995,12 @@
       <c r="C39" s="1">
         <v>44222.434027777781</v>
       </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>65.084446873087174</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -2963,6 +3011,12 @@
       </c>
       <c r="C40" s="1">
         <v>44229.90347222222</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E40" s="2">
+        <v>64.460062696726524</v>
       </c>
     </row>
   </sheetData>
@@ -2976,8 +3030,8 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38:A39"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3568,6 +3622,12 @@
       <c r="C38" s="1">
         <v>44215.482638888891</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>248.41137706173615</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -3578,6 +3638,12 @@
       </c>
       <c r="C39" s="1">
         <v>44229.421527777777</v>
+      </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>254.15565212542415</v>
       </c>
     </row>
   </sheetData>
@@ -3591,7 +3657,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A40"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4183,6 +4249,12 @@
       <c r="C38" s="1">
         <v>44215.5</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>52.363491489350224</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -4194,6 +4266,12 @@
       <c r="C39" s="1">
         <v>44222.463194444441</v>
       </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>54.098413011423467</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -4204,6 +4282,12 @@
       </c>
       <c r="C40" s="1">
         <v>44229.434027777781</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E40" s="2">
+        <v>54.752764122368603</v>
       </c>
     </row>
   </sheetData>
@@ -4216,8 +4300,8 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A40"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4808,6 +4892,12 @@
       <c r="C38" s="1">
         <v>44215.513888888891</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>52.55481583998899</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -4819,6 +4909,12 @@
       <c r="C39" s="1">
         <v>44222.524305555555</v>
       </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>47.749982553603786</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -4829,6 +4925,12 @@
       </c>
       <c r="C40" s="1">
         <v>44229.57916666667</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45.218251451867047</v>
       </c>
     </row>
   </sheetData>
@@ -4842,8 +4944,8 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A40"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5434,6 +5536,12 @@
       <c r="C38" s="1">
         <v>44215.536111111112</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>44.875003507587721</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -5445,6 +5553,12 @@
       <c r="C39" s="1">
         <v>44222.538888888892</v>
       </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>51.801539122318289</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -5455,6 +5569,12 @@
       </c>
       <c r="C40" s="1">
         <v>44229.59097222222</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E40" s="2">
+        <v>63.647882889890816</v>
       </c>
     </row>
   </sheetData>
@@ -5467,8 +5587,8 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A40"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6059,6 +6179,12 @@
       <c r="C38" s="1">
         <v>44215.541666666664</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>33.404635442140709</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -6070,6 +6196,12 @@
       <c r="C39" s="1">
         <v>44222.547222222223</v>
       </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>32.559971573282475</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -6080,6 +6212,12 @@
       </c>
       <c r="C40" s="1">
         <v>44229.599305555559</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E40" s="2">
+        <v>33.027292110241802</v>
       </c>
     </row>
   </sheetData>
@@ -6092,8 +6230,8 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A40"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6684,6 +6822,12 @@
       <c r="C38" s="1">
         <v>44215.5625</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>164.71836339372928</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -6695,6 +6839,12 @@
       <c r="C39" s="1">
         <v>44222.56527777778</v>
       </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>147.98878045469903</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -6705,6 +6855,12 @@
       </c>
       <c r="C40" s="1">
         <v>44229.497916666667</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E40" s="2">
+        <v>170.06235914006493</v>
       </c>
     </row>
   </sheetData>
@@ -6716,9 +6872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7312,6 +7468,12 @@
       <c r="C38" s="1">
         <v>44215.571527777778</v>
       </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>745.17040654164259</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
@@ -7322,6 +7484,12 @@
       </c>
       <c r="C39" s="1">
         <v>44229.474305555559</v>
+      </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>659.00866224346157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new data from sampling and scraping
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304B99DA-08FE-4691-B296-002861000773}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAB7472-58E8-4A05-8573-C23560961E17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32595" yWindow="3930" windowWidth="17280" windowHeight="8970" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29280" yWindow="495" windowWidth="17280" windowHeight="8970" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="9">
   <si>
     <t>chloride_mgL</t>
   </si>
@@ -935,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8232DBB5-5FD9-42B6-9357-9E7084957CC5}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1396,6 +1396,9 @@
       <c r="B28" s="1">
         <v>44243.427083333336</v>
       </c>
+      <c r="D28" s="4">
+        <v>44258</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1406,6 +1409,17 @@
       </c>
       <c r="C29" s="1">
         <v>44250.439583333333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44257.440972222219</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44257.440972222219</v>
       </c>
     </row>
   </sheetData>
@@ -1913,7 +1927,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="A33" sqref="A33:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2401,6 +2415,9 @@
       <c r="B33" s="1">
         <v>44244.642361111109</v>
       </c>
+      <c r="C33" s="1">
+        <v>44258</v>
+      </c>
       <c r="D33" s="2">
         <v>0</v>
       </c>
@@ -2412,6 +2429,9 @@
       <c r="B34" s="1">
         <v>44244.658333333333</v>
       </c>
+      <c r="C34" s="1">
+        <v>44258</v>
+      </c>
       <c r="D34" s="2">
         <v>5</v>
       </c>
@@ -2423,6 +2443,9 @@
       <c r="B35" s="1">
         <v>44244.655555555553</v>
       </c>
+      <c r="C35" s="1">
+        <v>44258</v>
+      </c>
       <c r="D35" s="2">
         <v>10</v>
       </c>
@@ -2434,6 +2457,9 @@
       <c r="B36" s="1">
         <v>44244.658333333333</v>
       </c>
+      <c r="C36" s="1">
+        <v>44258</v>
+      </c>
       <c r="D36" s="2">
         <v>15</v>
       </c>
@@ -2445,6 +2471,9 @@
       <c r="B37" s="1">
         <v>44244.652083333334</v>
       </c>
+      <c r="C37" s="1">
+        <v>44258</v>
+      </c>
       <c r="D37" s="2">
         <v>20</v>
       </c>
@@ -2455,6 +2484,9 @@
       </c>
       <c r="B38" s="1">
         <v>44244.636805555558</v>
+      </c>
+      <c r="C38" s="1">
+        <v>44258</v>
       </c>
       <c r="D38" s="2">
         <v>23.5</v>
@@ -2468,11 +2500,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3105,6 +3137,9 @@
       <c r="B41" s="1">
         <v>44243.440972222219</v>
       </c>
+      <c r="D41" s="4">
+        <v>44258</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -3115,6 +3150,23 @@
       </c>
       <c r="C42" s="1">
         <v>44250.455555555556</v>
+      </c>
+      <c r="D42" s="4">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44257.455555555556</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44257.455555555556</v>
+      </c>
+      <c r="D43" s="4">
+        <v>44258</v>
       </c>
     </row>
   </sheetData>
@@ -3125,11 +3177,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3748,6 +3800,9 @@
       <c r="B40" s="1">
         <v>44243.461805555555</v>
       </c>
+      <c r="D40" s="4">
+        <v>44258</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -3758,6 +3813,23 @@
       </c>
       <c r="C41" s="1">
         <v>44250.472222222219</v>
+      </c>
+      <c r="D41" s="4">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44257.473611111112</v>
+      </c>
+      <c r="C42" s="1">
+        <v>44257.473611111112</v>
+      </c>
+      <c r="D42" s="4">
+        <v>44258</v>
       </c>
     </row>
   </sheetData>
@@ -3767,11 +3839,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4408,6 +4480,9 @@
       <c r="B41" s="1">
         <v>44243.478472222225</v>
       </c>
+      <c r="D41" s="4">
+        <v>44257</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -4418,6 +4493,23 @@
       </c>
       <c r="C42" s="1">
         <v>44250.478472222225</v>
+      </c>
+      <c r="D42" s="4">
+        <v>44257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44257.489583333336</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44257.489583333336</v>
+      </c>
+      <c r="D43" s="4">
+        <v>44257</v>
       </c>
     </row>
   </sheetData>
@@ -4427,11 +4519,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5063,6 +5155,20 @@
         <v>45.218251451867047</v>
       </c>
     </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44257.544444444444</v>
+      </c>
+      <c r="C41" s="1">
+        <v>44257.544444444444</v>
+      </c>
+      <c r="D41" s="4">
+        <v>44258</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5071,11 +5177,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5711,6 +5817,9 @@
       <c r="B41" s="1">
         <v>44243.55</v>
       </c>
+      <c r="D41" s="4">
+        <v>44258</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -5721,6 +5830,23 @@
       </c>
       <c r="C42" s="1">
         <v>44250.53402777778</v>
+      </c>
+      <c r="D42" s="4">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44257.554861111108</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44257.554861111108</v>
+      </c>
+      <c r="D43" s="4">
+        <v>44258</v>
       </c>
     </row>
   </sheetData>
@@ -5730,11 +5856,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6370,6 +6496,9 @@
       <c r="B41" s="1">
         <v>44243.555555555555</v>
       </c>
+      <c r="D41" s="4">
+        <v>44258</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -6380,6 +6509,23 @@
       </c>
       <c r="C42" s="1">
         <v>44250.540277777778</v>
+      </c>
+      <c r="D42" s="4">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44257.560416666667</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44257.560416666667</v>
+      </c>
+      <c r="D43" s="4">
+        <v>44258</v>
       </c>
     </row>
   </sheetData>
@@ -6389,11 +6535,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7029,6 +7175,9 @@
       <c r="B41" s="1">
         <v>44243.569444444445</v>
       </c>
+      <c r="D41" s="4">
+        <v>44258</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -7039,6 +7188,23 @@
       </c>
       <c r="C42" s="1">
         <v>44250.554861111108</v>
+      </c>
+      <c r="D42" s="4">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44257.574999999997</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44257.574999999997</v>
+      </c>
+      <c r="D43" s="4">
+        <v>44258</v>
       </c>
     </row>
   </sheetData>
@@ -7048,11 +7214,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7674,6 +7840,9 @@
       <c r="B40" s="1">
         <v>44243.590277777781</v>
       </c>
+      <c r="D40" s="3">
+        <v>44258</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
@@ -7684,6 +7853,23 @@
       </c>
       <c r="C41" s="1">
         <v>44250.5625</v>
+      </c>
+      <c r="D41" s="3">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44257.583333333336</v>
+      </c>
+      <c r="C42" s="1">
+        <v>44257.583333333336</v>
+      </c>
+      <c r="D42" s="3">
+        <v>44258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new data from sampling
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFC05DD-6807-4197-9294-9554CC461369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2AA9DE-6815-49F7-BB65-CEDDF6CBC12D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32115" yWindow="3420" windowWidth="17280" windowHeight="8970" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="9">
   <si>
     <t>chloride_mgL</t>
   </si>
@@ -935,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8232DBB5-5FD9-42B6-9357-9E7084957CC5}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A30" sqref="A30:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1435,6 +1435,17 @@
       </c>
       <c r="E30" s="2">
         <v>205.27560785445988</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44264.453472222223</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44264.453472222223</v>
       </c>
     </row>
   </sheetData>
@@ -2533,11 +2544,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3211,6 +3222,17 @@
         <v>69.489219483720731</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44264.469444444447</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44264.469444444447</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3219,11 +3241,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3883,6 +3905,17 @@
         <v>303.69211263703858</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44264.490277777775</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44264.490277777775</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3890,11 +3923,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4572,6 +4605,17 @@
         <v>54.850965069449849</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44264.4375</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44264.4375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4579,11 +4623,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5232,6 +5276,17 @@
         <v>70.493956182742522</v>
       </c>
     </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44264.54583333333</v>
+      </c>
+      <c r="C42" s="1">
+        <v>44264.54583333333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5240,11 +5295,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5921,6 +5976,17 @@
         <v>52.629438733123131</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44264.561111111114</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44264.561111111114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5928,11 +5994,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6609,6 +6675,17 @@
         <v>45.273628317754493</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44264.572222222225</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44264.572222222225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6616,11 +6693,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7297,6 +7374,17 @@
         <v>270.02314761704781</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44264.587500000001</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44264.587500000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7304,11 +7392,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7971,6 +8059,17 @@
         <v>654.92546122180033</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44264.6</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44264.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
fixing color schemes and some mapping stuff
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2AA9DE-6815-49F7-BB65-CEDDF6CBC12D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00217FD-25FB-4A7E-95E8-3B9A3558A5C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32115" yWindow="3420" windowWidth="17280" windowHeight="8970" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="990" windowWidth="17280" windowHeight="8970" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="9">
   <si>
     <t>chloride_mgL</t>
   </si>
@@ -935,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8232DBB5-5FD9-42B6-9357-9E7084957CC5}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A31"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,6 +1446,28 @@
       </c>
       <c r="C31" s="1">
         <v>44264.453472222223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44271.411111111112</v>
+      </c>
+      <c r="C32" s="1">
+        <v>44271.411111111112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44278.401388888888</v>
+      </c>
+      <c r="C33" s="1">
+        <v>44278.401388888888</v>
       </c>
     </row>
   </sheetData>
@@ -2544,11 +2566,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3233,6 +3255,28 @@
         <v>44264.469444444447</v>
       </c>
     </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44271.425000000003</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44271.425000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44278.413194444445</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44278.413194444445</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3241,11 +3285,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3916,6 +3960,28 @@
         <v>44264.490277777775</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44271.440972222219</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44271.440972222219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44278.430555555555</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44278.430555555555</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3923,11 +3989,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4616,6 +4682,28 @@
         <v>44264.4375</v>
       </c>
     </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44271.440972222219</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44271.440972222219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44278.443055555559</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44278.443055555559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4623,682 +4711,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="1">
-        <v>43816.446527777778</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43846.481944444444</v>
-      </c>
-      <c r="D2" s="4">
-        <v>43865</v>
-      </c>
-      <c r="E2" s="2">
-        <v>53.197903408657218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
-        <v>43830.6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43846.480555555558</v>
-      </c>
-      <c r="D3" s="4">
-        <v>43865</v>
-      </c>
-      <c r="E3" s="2">
-        <v>38.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
-        <v>43836.445833333331</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43846.499305555553</v>
-      </c>
-      <c r="D4" s="4">
-        <v>43865</v>
-      </c>
-      <c r="E4" s="2">
-        <v>49.92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
-        <v>43844.618055555555</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43853.599999999999</v>
-      </c>
-      <c r="D5" s="4">
-        <v>43873</v>
-      </c>
-      <c r="E5" s="2">
-        <v>49.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
-        <v>43851.635416666664</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43853.593055555553</v>
-      </c>
-      <c r="D6" s="4">
-        <v>43873</v>
-      </c>
-      <c r="E6" s="2">
-        <v>50.652847736295882</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
-        <v>43858.624305555553</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43867.603472222225</v>
-      </c>
-      <c r="D7" s="4">
-        <v>43873</v>
-      </c>
-      <c r="E7" s="2">
-        <v>67.436843174760639</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
-        <v>43865.625</v>
-      </c>
-      <c r="C8" s="1">
-        <v>43874.590277777781</v>
-      </c>
-      <c r="D8" s="4">
-        <v>44104</v>
-      </c>
-      <c r="E8" s="2">
-        <v>53.295380894886883</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
-        <v>43872.621527777781</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43874.571527777778</v>
-      </c>
-      <c r="D9" s="4">
-        <v>44104</v>
-      </c>
-      <c r="E9" s="2">
-        <v>53.44165578732305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
-        <v>43879.630555555559</v>
-      </c>
-      <c r="C10" s="1">
-        <v>43881.571527777778</v>
-      </c>
-      <c r="D10" s="4">
-        <v>44104</v>
-      </c>
-      <c r="E10" s="2">
-        <v>50.625767083660222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
-        <v>43886.616666666669</v>
-      </c>
-      <c r="C11" s="1">
-        <v>43888.576388888891</v>
-      </c>
-      <c r="D11" s="4">
-        <v>44139</v>
-      </c>
-      <c r="E11" s="2">
-        <v>51.92872432371469</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
-        <v>43893.628472222219</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43895.569444444445</v>
-      </c>
-      <c r="D12" s="4">
-        <v>44144</v>
-      </c>
-      <c r="E12" s="2">
-        <v>52.001227118063163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <v>43900.574305555558</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43902</v>
-      </c>
-      <c r="D13" s="4">
-        <v>44145</v>
-      </c>
-      <c r="E13" s="2">
-        <v>36.005427589758071</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
-        <v>43906.40625</v>
-      </c>
-      <c r="D14" s="4">
-        <v>44117</v>
-      </c>
-      <c r="E14" s="2">
-        <v>46.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
-        <v>43999.487500000003</v>
-      </c>
-      <c r="D15" s="4">
-        <v>44138</v>
-      </c>
-      <c r="E15" s="2">
-        <v>34.918989526925834</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44012.433333333334</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44012.433333333334</v>
-      </c>
-      <c r="D16" s="4">
-        <v>44145</v>
-      </c>
-      <c r="E16" s="2">
-        <v>43.972274743186993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44012.43472222222</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44012.43472222222</v>
-      </c>
-      <c r="D17" s="4">
-        <v>44145</v>
-      </c>
-      <c r="E17" s="2">
-        <v>43.772969589609922</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1">
-        <v>44026.414583333331</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44026.414583333331</v>
-      </c>
-      <c r="D18" s="4">
-        <v>44145</v>
-      </c>
-      <c r="E18" s="2">
-        <v>28.481228144798386</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1">
-        <v>44026.414583333331</v>
-      </c>
-      <c r="C19" s="1">
-        <v>44026.414583333331</v>
-      </c>
-      <c r="D19" s="4">
-        <v>44145</v>
-      </c>
-      <c r="E19" s="2">
-        <v>28.272187668052851</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="1">
-        <v>44040.37222222222</v>
-      </c>
-      <c r="C20" s="1">
-        <v>44040.37222222222</v>
-      </c>
-      <c r="D20" s="4">
-        <v>44154</v>
-      </c>
-      <c r="E20" s="2">
-        <v>42.359894075705547</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="1">
-        <v>44040.37222222222</v>
-      </c>
-      <c r="C21" s="1">
-        <v>44040.37222222222</v>
-      </c>
-      <c r="D21" s="4">
-        <v>44154</v>
-      </c>
-      <c r="E21" s="2">
-        <v>42.100599065326627</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="1">
-        <v>44054.408333333333</v>
-      </c>
-      <c r="C22" s="1">
-        <v>44054.408333333333</v>
-      </c>
-      <c r="D22" s="4">
-        <v>44138</v>
-      </c>
-      <c r="E22" s="2">
-        <v>45.526267807475996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1">
-        <v>44054.408333333333</v>
-      </c>
-      <c r="C23" s="1">
-        <v>44054.408333333333</v>
-      </c>
-      <c r="D23" s="4">
-        <v>44138</v>
-      </c>
-      <c r="E23" s="2">
-        <v>45.573887601032474</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1">
-        <v>44069.425000000003</v>
-      </c>
-      <c r="D24" s="4">
-        <v>44138</v>
-      </c>
-      <c r="E24" s="2">
-        <v>48.312044984620705</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="1">
-        <v>44082.409722222219</v>
-      </c>
-      <c r="C25" s="1">
-        <v>44082.409722222219</v>
-      </c>
-      <c r="D25" s="4">
-        <v>44144</v>
-      </c>
-      <c r="E25" s="2">
-        <v>45.675622792676322</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="1">
-        <v>44082.409722222219</v>
-      </c>
-      <c r="C26" s="1">
-        <v>44082.409722222219</v>
-      </c>
-      <c r="D26" s="4">
-        <v>44144</v>
-      </c>
-      <c r="E26" s="2">
-        <v>45.583048013439402</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="1">
-        <v>44096.418749999997</v>
-      </c>
-      <c r="C27" s="1">
-        <v>44096.418749999997</v>
-      </c>
-      <c r="D27" s="4">
-        <v>44139</v>
-      </c>
-      <c r="E27" s="2">
-        <v>47.418022535560965</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="1">
-        <v>44110.392361111109</v>
-      </c>
-      <c r="C28" s="1">
-        <v>44110.392361111109</v>
-      </c>
-      <c r="D28" s="4">
-        <v>44138</v>
-      </c>
-      <c r="E28" s="2">
-        <v>47.829696742709331</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="1">
-        <v>44126.410416666666</v>
-      </c>
-      <c r="D29" s="4">
-        <v>44139</v>
-      </c>
-      <c r="E29" s="2">
-        <v>43.990439619876931</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="1">
-        <v>44134.345138888886</v>
-      </c>
-      <c r="C30" s="1">
-        <v>44134.345138888886</v>
-      </c>
-      <c r="D30" s="4">
-        <v>44139</v>
-      </c>
-      <c r="E30" s="2">
-        <v>39.404694761818924</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="1">
-        <v>44152.529166666667</v>
-      </c>
-      <c r="C31" s="1">
-        <v>44152.529166666667</v>
-      </c>
-      <c r="D31" s="4">
-        <v>44154</v>
-      </c>
-      <c r="E31" s="2">
-        <v>42.971316631885529</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="1">
-        <v>44159.513194444444</v>
-      </c>
-      <c r="C32" s="1">
-        <v>44159.513194444444</v>
-      </c>
-      <c r="D32" s="4">
-        <v>44175</v>
-      </c>
-      <c r="E32" s="2">
-        <v>49.139387608397101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="1">
-        <v>44173.482638888891</v>
-      </c>
-      <c r="C33" s="1">
-        <v>44169.482638888891</v>
-      </c>
-      <c r="D33" s="4">
-        <v>44175</v>
-      </c>
-      <c r="E33" s="2">
-        <v>50.508592344335561</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="1">
-        <v>44180.623611111114</v>
-      </c>
-      <c r="C34" s="1">
-        <v>44180.623611111114</v>
-      </c>
-      <c r="D34" s="4">
-        <v>44182</v>
-      </c>
-      <c r="E34" s="2">
-        <v>50.235612939987639</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="1">
-        <v>44194.457638888889</v>
-      </c>
-      <c r="C35" s="1">
-        <v>44194.457638888889</v>
-      </c>
-      <c r="D35" s="4">
-        <v>44203</v>
-      </c>
-      <c r="E35" s="2">
-        <v>47.043545551602335</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="1">
-        <v>44201.527777777781</v>
-      </c>
-      <c r="C36" s="1">
-        <v>44201.527777777781</v>
-      </c>
-      <c r="D36" s="4">
-        <v>44203</v>
-      </c>
-      <c r="E36" s="2">
-        <v>42.887212448968732</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="1">
-        <v>44208.549305555556</v>
-      </c>
-      <c r="C37" s="1">
-        <v>44208.549305555556</v>
-      </c>
-      <c r="D37" s="4">
-        <v>44210</v>
-      </c>
-      <c r="E37" s="2">
-        <v>46.519491182570441</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="1">
-        <v>44215.513888888891</v>
-      </c>
-      <c r="C38" s="1">
-        <v>44215.513888888891</v>
-      </c>
-      <c r="D38" s="4">
-        <v>44238</v>
-      </c>
-      <c r="E38" s="2">
-        <v>52.55481583998899</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="1">
-        <v>44222.524305555555</v>
-      </c>
-      <c r="C39" s="1">
-        <v>44222.524305555555</v>
-      </c>
-      <c r="D39" s="4">
-        <v>44238</v>
-      </c>
-      <c r="E39" s="2">
-        <v>47.749982553603786</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="1">
-        <v>44229.57916666667</v>
-      </c>
-      <c r="C40" s="1">
-        <v>44229.57916666667</v>
-      </c>
-      <c r="D40" s="4">
-        <v>44238</v>
-      </c>
-      <c r="E40" s="2">
-        <v>45.218251451867047</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="1">
-        <v>44257.544444444444</v>
-      </c>
-      <c r="C41" s="1">
-        <v>44257.544444444444</v>
-      </c>
-      <c r="D41" s="4">
-        <v>44258</v>
-      </c>
-      <c r="E41" s="2">
-        <v>70.493956182742522</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="1">
-        <v>44264.54583333333</v>
-      </c>
-      <c r="C42" s="1">
-        <v>44264.54583333333</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -5330,6 +4746,700 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
+        <v>43816.446527777778</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43846.481944444444</v>
+      </c>
+      <c r="D2" s="4">
+        <v>43865</v>
+      </c>
+      <c r="E2" s="2">
+        <v>53.197903408657218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <v>43830.6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43846.480555555558</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43865</v>
+      </c>
+      <c r="E3" s="2">
+        <v>38.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>43836.445833333331</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43846.499305555553</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43865</v>
+      </c>
+      <c r="E4" s="2">
+        <v>49.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>43844.618055555555</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43853.599999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43873</v>
+      </c>
+      <c r="E5" s="2">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>43851.635416666664</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43853.593055555553</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43873</v>
+      </c>
+      <c r="E6" s="2">
+        <v>50.652847736295882</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>43858.624305555553</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43867.603472222225</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43873</v>
+      </c>
+      <c r="E7" s="2">
+        <v>67.436843174760639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>43865.625</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43874.590277777781</v>
+      </c>
+      <c r="D8" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E8" s="2">
+        <v>53.295380894886883</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>43872.621527777781</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43874.571527777778</v>
+      </c>
+      <c r="D9" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E9" s="2">
+        <v>53.44165578732305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>43879.630555555559</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43881.571527777778</v>
+      </c>
+      <c r="D10" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E10" s="2">
+        <v>50.625767083660222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>43886.616666666669</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43888.576388888891</v>
+      </c>
+      <c r="D11" s="4">
+        <v>44139</v>
+      </c>
+      <c r="E11" s="2">
+        <v>51.92872432371469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>43893.628472222219</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43895.569444444445</v>
+      </c>
+      <c r="D12" s="4">
+        <v>44144</v>
+      </c>
+      <c r="E12" s="2">
+        <v>52.001227118063163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>43900.574305555558</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43902</v>
+      </c>
+      <c r="D13" s="4">
+        <v>44145</v>
+      </c>
+      <c r="E13" s="2">
+        <v>36.005427589758071</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>43906.40625</v>
+      </c>
+      <c r="D14" s="4">
+        <v>44117</v>
+      </c>
+      <c r="E14" s="2">
+        <v>46.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>43999.487500000003</v>
+      </c>
+      <c r="D15" s="4">
+        <v>44138</v>
+      </c>
+      <c r="E15" s="2">
+        <v>34.918989526925834</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44012.433333333334</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44012.433333333334</v>
+      </c>
+      <c r="D16" s="4">
+        <v>44145</v>
+      </c>
+      <c r="E16" s="2">
+        <v>43.972274743186993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44012.43472222222</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44012.43472222222</v>
+      </c>
+      <c r="D17" s="4">
+        <v>44145</v>
+      </c>
+      <c r="E17" s="2">
+        <v>43.772969589609922</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44026.414583333331</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44026.414583333331</v>
+      </c>
+      <c r="D18" s="4">
+        <v>44145</v>
+      </c>
+      <c r="E18" s="2">
+        <v>28.481228144798386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44026.414583333331</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44026.414583333331</v>
+      </c>
+      <c r="D19" s="4">
+        <v>44145</v>
+      </c>
+      <c r="E19" s="2">
+        <v>28.272187668052851</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44040.37222222222</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44040.37222222222</v>
+      </c>
+      <c r="D20" s="4">
+        <v>44154</v>
+      </c>
+      <c r="E20" s="2">
+        <v>42.359894075705547</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44040.37222222222</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44040.37222222222</v>
+      </c>
+      <c r="D21" s="4">
+        <v>44154</v>
+      </c>
+      <c r="E21" s="2">
+        <v>42.100599065326627</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44054.408333333333</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44054.408333333333</v>
+      </c>
+      <c r="D22" s="4">
+        <v>44138</v>
+      </c>
+      <c r="E22" s="2">
+        <v>45.526267807475996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44054.408333333333</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44054.408333333333</v>
+      </c>
+      <c r="D23" s="4">
+        <v>44138</v>
+      </c>
+      <c r="E23" s="2">
+        <v>45.573887601032474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>44069.425000000003</v>
+      </c>
+      <c r="D24" s="4">
+        <v>44138</v>
+      </c>
+      <c r="E24" s="2">
+        <v>48.312044984620705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44082.409722222219</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44082.409722222219</v>
+      </c>
+      <c r="D25" s="4">
+        <v>44144</v>
+      </c>
+      <c r="E25" s="2">
+        <v>45.675622792676322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44082.409722222219</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44082.409722222219</v>
+      </c>
+      <c r="D26" s="4">
+        <v>44144</v>
+      </c>
+      <c r="E26" s="2">
+        <v>45.583048013439402</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44096.418749999997</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44096.418749999997</v>
+      </c>
+      <c r="D27" s="4">
+        <v>44139</v>
+      </c>
+      <c r="E27" s="2">
+        <v>47.418022535560965</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44110.392361111109</v>
+      </c>
+      <c r="C28" s="1">
+        <v>44110.392361111109</v>
+      </c>
+      <c r="D28" s="4">
+        <v>44138</v>
+      </c>
+      <c r="E28" s="2">
+        <v>47.829696742709331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>44126.410416666666</v>
+      </c>
+      <c r="D29" s="4">
+        <v>44139</v>
+      </c>
+      <c r="E29" s="2">
+        <v>43.990439619876931</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44134.345138888886</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44134.345138888886</v>
+      </c>
+      <c r="D30" s="4">
+        <v>44139</v>
+      </c>
+      <c r="E30" s="2">
+        <v>39.404694761818924</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44152.529166666667</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44152.529166666667</v>
+      </c>
+      <c r="D31" s="4">
+        <v>44154</v>
+      </c>
+      <c r="E31" s="2">
+        <v>42.971316631885529</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44159.513194444444</v>
+      </c>
+      <c r="C32" s="1">
+        <v>44159.513194444444</v>
+      </c>
+      <c r="D32" s="4">
+        <v>44175</v>
+      </c>
+      <c r="E32" s="2">
+        <v>49.139387608397101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44173.482638888891</v>
+      </c>
+      <c r="C33" s="1">
+        <v>44169.482638888891</v>
+      </c>
+      <c r="D33" s="4">
+        <v>44175</v>
+      </c>
+      <c r="E33" s="2">
+        <v>50.508592344335561</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44180.623611111114</v>
+      </c>
+      <c r="C34" s="1">
+        <v>44180.623611111114</v>
+      </c>
+      <c r="D34" s="4">
+        <v>44182</v>
+      </c>
+      <c r="E34" s="2">
+        <v>50.235612939987639</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44194.457638888889</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44194.457638888889</v>
+      </c>
+      <c r="D35" s="4">
+        <v>44203</v>
+      </c>
+      <c r="E35" s="2">
+        <v>47.043545551602335</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44201.527777777781</v>
+      </c>
+      <c r="C36" s="1">
+        <v>44201.527777777781</v>
+      </c>
+      <c r="D36" s="4">
+        <v>44203</v>
+      </c>
+      <c r="E36" s="2">
+        <v>42.887212448968732</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44208.549305555556</v>
+      </c>
+      <c r="C37" s="1">
+        <v>44208.549305555556</v>
+      </c>
+      <c r="D37" s="4">
+        <v>44210</v>
+      </c>
+      <c r="E37" s="2">
+        <v>46.519491182570441</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44215.513888888891</v>
+      </c>
+      <c r="C38" s="1">
+        <v>44215.513888888891</v>
+      </c>
+      <c r="D38" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E38" s="2">
+        <v>52.55481583998899</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44222.524305555555</v>
+      </c>
+      <c r="C39" s="1">
+        <v>44222.524305555555</v>
+      </c>
+      <c r="D39" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E39" s="2">
+        <v>47.749982553603786</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44229.57916666667</v>
+      </c>
+      <c r="C40" s="1">
+        <v>44229.57916666667</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44238</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45.218251451867047</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44257.544444444444</v>
+      </c>
+      <c r="C41" s="1">
+        <v>44257.544444444444</v>
+      </c>
+      <c r="D41" s="4">
+        <v>44258</v>
+      </c>
+      <c r="E41" s="2">
+        <v>70.493956182742522</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44264.54583333333</v>
+      </c>
+      <c r="C42" s="1">
+        <v>44264.54583333333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44271.526388888888</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44271.526388888888</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44278.493750000001</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44278.493750000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="1">
         <v>43816.631249999999</v>
       </c>
       <c r="C2" s="1">
@@ -5985,6 +6095,28 @@
       </c>
       <c r="C44" s="1">
         <v>44264.561111111114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44271.543749999997</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44271.543749999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44278.50277777778</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44278.50277777778</v>
       </c>
     </row>
   </sheetData>
@@ -5994,11 +6126,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6686,6 +6818,28 @@
         <v>44264.572222222225</v>
       </c>
     </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44271.552083333336</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44271.552083333336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44278.509722222225</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44278.509722222225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6693,11 +6847,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7385,6 +7539,28 @@
         <v>44264.587500000001</v>
       </c>
     </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44271.567361111112</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44271.567361111112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44278.525000000001</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44278.525000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7392,11 +7568,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8070,6 +8246,28 @@
         <v>44264.6</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44271.579861111109</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44271.579861111109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44278.53402777778</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44278.53402777778</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
continuing to work on salt results
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8C2241-8233-4895-A409-042632F6B8A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F551A5-2E94-458E-AF8E-87EE90EC1CBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3756" yWindow="1452" windowWidth="13836" windowHeight="7176" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30675" yWindow="1935" windowWidth="17280" windowHeight="8970" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <sheet name="DC" sheetId="6" r:id="rId7"/>
     <sheet name="PBMS" sheetId="7" r:id="rId8"/>
     <sheet name="PBSF" sheetId="8" r:id="rId9"/>
-    <sheet name="MO" sheetId="11" r:id="rId10"/>
-    <sheet name="ME" sheetId="10" r:id="rId11"/>
+    <sheet name="ME" sheetId="10" r:id="rId10"/>
+    <sheet name="MO" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="10">
   <si>
     <t>chloride_mgL</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Whatman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1498,11 +1501,656 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3A990-AAD2-449A-8315-183C290E8A9C}">
+  <dimension ref="A1:F44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39:D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43888.587500000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44144</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>53.130226107507411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43888.586805555555</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44144</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>51.817612674289492</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43888.588888888888</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44144</v>
+      </c>
+      <c r="D4" s="2">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2">
+        <v>49.223856351539915</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43888.59097222222</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44144</v>
+      </c>
+      <c r="D5" s="2">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2">
+        <v>50.426076982957802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43888.59097222222</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44144</v>
+      </c>
+      <c r="D6" s="2">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2">
+        <v>52.296120550875209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43888.593055555553</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44144</v>
+      </c>
+      <c r="D7" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>52.45229600086676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43922.416666666664</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44112.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>50.173757230541511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43922.416666666664</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44112.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>50.52387736111401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>44028.5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>49.617549353114299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44028.5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>50.830047564510913</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44028.5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2">
+        <v>51.196534374320564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44028.5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2">
+        <v>51.129040054470337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44028.5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D14" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>51.192265821645336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44055.5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>49.425633306154914</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44055.5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>49.228023352011775</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44055.5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D17" s="2">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>50.168292735987571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44055.5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D18" s="2">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2">
+        <v>50.824418978963017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44055.5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D19" s="2">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2">
+        <v>50.766265311623648</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44055.5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D20" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>50.572698527752237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44106.5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>50.011343110286838</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44106.5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <v>49.697295633396593</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44106.5</v>
+      </c>
+      <c r="C23" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2">
+        <v>49.644812828587192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>44106.5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D24" s="2">
+        <v>15</v>
+      </c>
+      <c r="E24" s="2">
+        <v>50.003064275759328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44106.5</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D25" s="2">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2">
+        <v>50.22995948966247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44106.5</v>
+      </c>
+      <c r="C26" s="1">
+        <v>42290</v>
+      </c>
+      <c r="D26" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>50.260498492386141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44169.5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>51.410427807542867</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44169.5</v>
+      </c>
+      <c r="C28" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2">
+        <v>51.348805574865771</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44169.5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <v>51.481335951620999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44169.5</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D30" s="2">
+        <v>15</v>
+      </c>
+      <c r="E30" s="2">
+        <v>51.617993400110031</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44169.5</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D31" s="2">
+        <v>20</v>
+      </c>
+      <c r="E31" s="2">
+        <v>51.786372669433376</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>44169.5</v>
+      </c>
+      <c r="C32" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D32" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>51.783703330638637</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>44244.642361111109</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44244.642361111109</v>
+      </c>
+      <c r="C33" s="1">
+        <v>44258</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>54.089643595283988</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>44244.658333333333</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44244.658333333333</v>
+      </c>
+      <c r="C34" s="1">
+        <v>44258</v>
+      </c>
+      <c r="D34" s="2">
+        <v>5</v>
+      </c>
+      <c r="E34" s="2">
+        <v>50.584270907419885</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>44244.655555555553</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44244.655555555553</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44258</v>
+      </c>
+      <c r="D35" s="2">
+        <v>10</v>
+      </c>
+      <c r="E35" s="2">
+        <v>50.72963979570531</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>44244.658333333333</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44244.658333333333</v>
+      </c>
+      <c r="C36" s="1">
+        <v>44258</v>
+      </c>
+      <c r="D36" s="2">
+        <v>15</v>
+      </c>
+      <c r="E36" s="2">
+        <v>51.383869600333632</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>44244.652083333334</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44244.652083333334</v>
+      </c>
+      <c r="C37" s="1">
+        <v>44258</v>
+      </c>
+      <c r="D37" s="2">
+        <v>20</v>
+      </c>
+      <c r="E37" s="2">
+        <v>49.691411215719029</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>44244.636805555558</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44244.636805555558</v>
+      </c>
+      <c r="C38" s="1">
+        <v>44258</v>
+      </c>
+      <c r="D38" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E38" s="2">
+        <v>48.675978752108492</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>44302.395833333336</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>44302.394444444442</v>
+      </c>
+      <c r="D40" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>44302.390972222223</v>
+      </c>
+      <c r="D41" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>44302.388194444444</v>
+      </c>
+      <c r="D42" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>44302.383333333331</v>
+      </c>
+      <c r="D43" s="2">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>44302.379861111112</v>
+      </c>
+      <c r="D44" s="2">
+        <v>23.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D91DE40-05E6-4B37-9CD8-EC471F027E06}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1640,7 +2288,7 @@
       <c r="C8" s="1">
         <v>42290</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8" s="2">
@@ -1654,7 +2302,7 @@
       <c r="C9" s="1">
         <v>42290</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>4</v>
       </c>
       <c r="E9" s="2">
@@ -1668,7 +2316,7 @@
       <c r="C10" s="1">
         <v>42290</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>8</v>
       </c>
       <c r="E10" s="2">
@@ -1682,7 +2330,7 @@
       <c r="C11" s="1">
         <v>42290</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>12</v>
       </c>
       <c r="E11" s="2">
@@ -1696,7 +2344,7 @@
       <c r="C12" s="1">
         <v>42290</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>16</v>
       </c>
       <c r="E12" s="2">
@@ -1710,7 +2358,7 @@
       <c r="C13" s="1">
         <v>42290</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>20</v>
       </c>
       <c r="E13" s="2">
@@ -2037,600 +2685,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3A990-AAD2-449A-8315-183C290E8A9C}">
-  <dimension ref="A1:E38"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33:E38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43888.587500000001</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44144</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>53.130226107507411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43888.586805555555</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44144</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2">
-        <v>51.817612674289492</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43888.588888888888</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44144</v>
-      </c>
-      <c r="D4" s="2">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2">
-        <v>49.223856351539915</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43888.59097222222</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44144</v>
-      </c>
-      <c r="D5" s="2">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2">
-        <v>50.426076982957802</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43888.59097222222</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44144</v>
-      </c>
-      <c r="D6" s="2">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2">
-        <v>52.296120550875209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>43886.5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43888.593055555553</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44144</v>
-      </c>
-      <c r="D7" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>52.45229600086676</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>43922.416666666664</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44112.5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>50.173757230541511</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>43922.416666666664</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44112.5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>50.52387736111401</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>44028.5</v>
-      </c>
-      <c r="C10" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>49.617549353114299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>44028.5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D11" s="2">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2">
-        <v>50.830047564510913</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>44028.5</v>
-      </c>
-      <c r="C12" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D12" s="2">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2">
-        <v>51.196534374320564</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>44028.5</v>
-      </c>
-      <c r="C13" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D13" s="2">
-        <v>20</v>
-      </c>
-      <c r="E13" s="2">
-        <v>51.129040054470337</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>44028.5</v>
-      </c>
-      <c r="C14" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D14" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E14" s="2">
-        <v>51.192265821645336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>44055.5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>49.425633306154914</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>44055.5</v>
-      </c>
-      <c r="C16" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>49.228023352011775</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>44055.5</v>
-      </c>
-      <c r="C17" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D17" s="2">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2">
-        <v>50.168292735987571</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>44055.5</v>
-      </c>
-      <c r="C18" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D18" s="2">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2">
-        <v>50.824418978963017</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>44055.5</v>
-      </c>
-      <c r="C19" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D19" s="2">
-        <v>20</v>
-      </c>
-      <c r="E19" s="2">
-        <v>50.766265311623648</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>44055.5</v>
-      </c>
-      <c r="C20" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D20" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>50.572698527752237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>44106.5</v>
-      </c>
-      <c r="C21" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>50.011343110286838</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>44106.5</v>
-      </c>
-      <c r="C22" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>49.697295633396593</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>44106.5</v>
-      </c>
-      <c r="C23" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D23" s="2">
-        <v>10</v>
-      </c>
-      <c r="E23" s="2">
-        <v>49.644812828587192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>44106.5</v>
-      </c>
-      <c r="C24" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D24" s="2">
-        <v>15</v>
-      </c>
-      <c r="E24" s="2">
-        <v>50.003064275759328</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>44106.5</v>
-      </c>
-      <c r="C25" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D25" s="2">
-        <v>20</v>
-      </c>
-      <c r="E25" s="2">
-        <v>50.22995948966247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>44106.5</v>
-      </c>
-      <c r="C26" s="1">
-        <v>42290</v>
-      </c>
-      <c r="D26" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>50.260498492386141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>44169.5</v>
-      </c>
-      <c r="C27" s="1">
-        <v>44175</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>51.410427807542867</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>44169.5</v>
-      </c>
-      <c r="C28" s="1">
-        <v>44175</v>
-      </c>
-      <c r="D28" s="2">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>51.348805574865771</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>44169.5</v>
-      </c>
-      <c r="C29" s="1">
-        <v>44175</v>
-      </c>
-      <c r="D29" s="2">
-        <v>10</v>
-      </c>
-      <c r="E29" s="2">
-        <v>51.481335951620999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>44169.5</v>
-      </c>
-      <c r="C30" s="1">
-        <v>44175</v>
-      </c>
-      <c r="D30" s="2">
-        <v>15</v>
-      </c>
-      <c r="E30" s="2">
-        <v>51.617993400110031</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>44169.5</v>
-      </c>
-      <c r="C31" s="1">
-        <v>44175</v>
-      </c>
-      <c r="D31" s="2">
-        <v>20</v>
-      </c>
-      <c r="E31" s="2">
-        <v>51.786372669433376</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>44169.5</v>
-      </c>
-      <c r="C32" s="1">
-        <v>44175</v>
-      </c>
-      <c r="D32" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E32" s="2">
-        <v>51.783703330638637</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>44244.642361111109</v>
-      </c>
-      <c r="B33" s="1">
-        <v>44244.642361111109</v>
-      </c>
-      <c r="C33" s="1">
-        <v>44258</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>54.089643595283988</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>44244.658333333333</v>
-      </c>
-      <c r="B34" s="1">
-        <v>44244.658333333333</v>
-      </c>
-      <c r="C34" s="1">
-        <v>44258</v>
-      </c>
-      <c r="D34" s="2">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2">
-        <v>50.584270907419885</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>44244.655555555553</v>
-      </c>
-      <c r="B35" s="1">
-        <v>44244.655555555553</v>
-      </c>
-      <c r="C35" s="1">
-        <v>44258</v>
-      </c>
-      <c r="D35" s="2">
-        <v>10</v>
-      </c>
-      <c r="E35" s="2">
-        <v>50.72963979570531</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>44244.658333333333</v>
-      </c>
-      <c r="B36" s="1">
-        <v>44244.658333333333</v>
-      </c>
-      <c r="C36" s="1">
-        <v>44258</v>
-      </c>
-      <c r="D36" s="2">
-        <v>15</v>
-      </c>
-      <c r="E36" s="2">
-        <v>51.383869600333632</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>44244.652083333334</v>
-      </c>
-      <c r="B37" s="1">
-        <v>44244.652083333334</v>
-      </c>
-      <c r="C37" s="1">
-        <v>44258</v>
-      </c>
-      <c r="D37" s="2">
-        <v>20</v>
-      </c>
-      <c r="E37" s="2">
-        <v>49.691411215719029</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>44244.636805555558</v>
-      </c>
-      <c r="B38" s="1">
-        <v>44244.636805555558</v>
-      </c>
-      <c r="C38" s="1">
-        <v>44258</v>
-      </c>
-      <c r="D38" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E38" s="2">
-        <v>48.675978752108492</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
more figs for presentation work
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F551A5-2E94-458E-AF8E-87EE90EC1CBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A176FA3-AEF3-4F96-B2F5-FB95BA2D6146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30675" yWindow="1935" windowWidth="17280" windowHeight="8970" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -1504,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3A990-AAD2-449A-8315-183C290E8A9C}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1658,7 +1658,7 @@
         <v>44112.5</v>
       </c>
       <c r="D9" s="2">
-        <v>23.5</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2">
         <v>50.52387736111401</v>

</xml_diff>

<commit_message>
new chloride data from lab runs this week
</commit_message>
<xml_diff>
--- a/Data/chloride_lab.xlsx
+++ b/Data/chloride_lab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A176FA3-AEF3-4F96-B2F5-FB95BA2D6146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27384557-681F-496E-BE8C-8ACBAEB86D61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="12" r:id="rId1"/>
@@ -77,10 +77,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="mm\-dd\-yyyy"/>
     <numFmt numFmtId="166" formatCode="mm\-dd\-yyyy\ "/>
+    <numFmt numFmtId="167" formatCode="0.0000&quot;  &quot;"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -565,7 +566,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -583,6 +584,7 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8232DBB5-5FD9-42B6-9357-9E7084957CC5}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1450,6 +1452,12 @@
       <c r="C31" s="1">
         <v>44264.453472222223</v>
       </c>
+      <c r="D31" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E31" s="2">
+        <v>190.18578318143318</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1461,8 +1469,14 @@
       <c r="C32" s="1">
         <v>44271.411111111112</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E32" s="2">
+        <v>142.92456943931035</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1472,8 +1486,14 @@
       <c r="C33" s="1">
         <v>44278.401388888888</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E33" s="2">
+        <v>155.85878518378513</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1483,8 +1503,14 @@
       <c r="C34" s="1">
         <v>44285.384027777778</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E34" s="2">
+        <v>163.78931764821081</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1493,6 +1519,12 @@
       </c>
       <c r="C35" s="1">
         <v>44296.418749999997</v>
+      </c>
+      <c r="D35" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E35" s="2">
+        <v>149.16085708008623</v>
       </c>
     </row>
   </sheetData>
@@ -1504,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3A990-AAD2-449A-8315-183C290E8A9C}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1658,7 +1690,7 @@
         <v>44112.5</v>
       </c>
       <c r="D9" s="2">
-        <v>24</v>
+        <v>23.5</v>
       </c>
       <c r="E9" s="2">
         <v>50.52387736111401</v>
@@ -2095,6 +2127,9 @@
       <c r="D39" s="2">
         <v>0</v>
       </c>
+      <c r="E39" s="2">
+        <v>50.417492169066229</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
@@ -2103,6 +2138,9 @@
       <c r="D40" s="2">
         <v>5</v>
       </c>
+      <c r="E40" s="2">
+        <v>50.476847816961254</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -2111,6 +2149,9 @@
       <c r="D41" s="2">
         <v>10</v>
       </c>
+      <c r="E41" s="2">
+        <v>50.448725368006372</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -2119,6 +2160,9 @@
       <c r="D42" s="2">
         <v>15</v>
       </c>
+      <c r="E42" s="2">
+        <v>50.345078277534625</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -2127,6 +2171,9 @@
       <c r="D43" s="2">
         <v>20</v>
       </c>
+      <c r="E43" s="2">
+        <v>50.365551997511844</v>
+      </c>
       <c r="F43" t="s">
         <v>9</v>
       </c>
@@ -2137,6 +2184,9 @@
       </c>
       <c r="D44" s="2">
         <v>23.5</v>
+      </c>
+      <c r="E44" s="2">
+        <v>50.433703667235179</v>
       </c>
     </row>
   </sheetData>
@@ -2150,7 +2200,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2642,45 +2692,63 @@
       <c r="D32" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="2">
+        <v>69.27940178255723</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44296.304166666669</v>
       </c>
       <c r="D33" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="2">
+        <v>69.235461098719682</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44296.302083333336</v>
       </c>
       <c r="D34" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="2">
+        <v>69.155059871482635</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44296.299305555556</v>
       </c>
       <c r="D35" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="2">
+        <v>69.262376099617626</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>44296.296527777777</v>
       </c>
       <c r="D36" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="2">
+        <v>69.249871844740682</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>44296.293749999997</v>
       </c>
       <c r="D37" s="2">
         <v>20</v>
+      </c>
+      <c r="E37" s="2">
+        <v>69.274492094977646</v>
       </c>
     </row>
   </sheetData>
@@ -2694,7 +2762,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3378,6 +3446,12 @@
       <c r="C44" s="1">
         <v>44264.469444444447</v>
       </c>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>65.937008549019509</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -3389,6 +3463,12 @@
       <c r="C45" s="1">
         <v>44271.425000000003</v>
       </c>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>64.916775896877226</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -3400,6 +3480,12 @@
       <c r="C46" s="1">
         <v>44278.413194444445</v>
       </c>
+      <c r="D46" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E46" s="2">
+        <v>62.966852946121989</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -3411,6 +3497,12 @@
       <c r="C47" s="1">
         <v>44285.395833333336</v>
       </c>
+      <c r="D47" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E47" s="2">
+        <v>73.022915532738907</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -3421,6 +3513,12 @@
       </c>
       <c r="C48" s="1">
         <v>44296.442361111112</v>
+      </c>
+      <c r="D48" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E48" s="2">
+        <v>69.055096765022938</v>
       </c>
     </row>
   </sheetData>
@@ -3435,7 +3533,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4105,6 +4203,12 @@
       <c r="C43" s="1">
         <v>44264.490277777775</v>
       </c>
+      <c r="D43" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E43" s="2">
+        <v>167.03126705319542</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -4116,6 +4220,12 @@
       <c r="C44" s="1">
         <v>44271.440972222219</v>
       </c>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>314.03501463113281</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -4127,6 +4237,12 @@
       <c r="C45" s="1">
         <v>44278.430555555555</v>
       </c>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>175.58548849981761</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -4138,6 +4254,12 @@
       <c r="C46" s="1">
         <v>44285.415277777778</v>
       </c>
+      <c r="D46" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E46" s="2">
+        <v>172.44891685623841</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -4148,6 +4270,12 @@
       </c>
       <c r="C47" s="1">
         <v>44296.474999999999</v>
+      </c>
+      <c r="D47" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E47" s="2">
+        <v>160.20135581791536</v>
       </c>
     </row>
   </sheetData>
@@ -4161,7 +4289,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4849,6 +4977,12 @@
       <c r="C44" s="1">
         <v>44264.4375</v>
       </c>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>53.842873561988284</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -4860,6 +4994,12 @@
       <c r="C45" s="1">
         <v>44271.440972222219</v>
       </c>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>56.919806316788438</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -4871,6 +5011,12 @@
       <c r="C46" s="1">
         <v>44278.443055555559</v>
       </c>
+      <c r="D46" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E46" s="2">
+        <v>54.678247898757647</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -4882,6 +5028,12 @@
       <c r="C47" s="1">
         <v>44285.429166666669</v>
       </c>
+      <c r="D47" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E47" s="2">
+        <v>55.134628724531538</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -4892,6 +5044,12 @@
       </c>
       <c r="C48" s="1">
         <v>44296.490972222222</v>
+      </c>
+      <c r="D48" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E48" s="2">
+        <v>51.410710930616098</v>
       </c>
     </row>
   </sheetData>
@@ -4905,7 +5063,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5564,6 +5722,12 @@
       <c r="C42" s="1">
         <v>44264.54583333333</v>
       </c>
+      <c r="D42" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E42" s="2">
+        <v>47.290463656411802</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -5575,6 +5739,12 @@
       <c r="C43" s="1">
         <v>44271.526388888888</v>
       </c>
+      <c r="D43" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E43" s="2">
+        <v>49.154552107291416</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -5586,6 +5756,12 @@
       <c r="C44" s="1">
         <v>44278.493750000001</v>
       </c>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>50.097908502477658</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -5597,6 +5773,12 @@
       <c r="C45" s="1">
         <v>44285.497916666667</v>
       </c>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>53.292198784936538</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -5607,6 +5789,12 @@
       </c>
       <c r="C46" s="1">
         <v>44296.509722222225</v>
+      </c>
+      <c r="D46" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E46" s="2">
+        <v>50.3128453694491</v>
       </c>
     </row>
   </sheetData>
@@ -5620,8 +5808,8 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6308,6 +6496,12 @@
       <c r="C44" s="1">
         <v>44264.561111111114</v>
       </c>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>32.666327290526567</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -6319,6 +6513,12 @@
       <c r="C45" s="1">
         <v>44271.543749999997</v>
       </c>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>46.668096397221682</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -6330,6 +6530,12 @@
       <c r="C46" s="1">
         <v>44278.50277777778</v>
       </c>
+      <c r="D46" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E46" s="2">
+        <v>43.779491029297475</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -6341,6 +6547,12 @@
       <c r="C47" s="1">
         <v>44285.507638888892</v>
       </c>
+      <c r="D47" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E47" s="2">
+        <v>42.987025029333239</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -6351,6 +6563,12 @@
       </c>
       <c r="C48" s="1">
         <v>44296.520833333336</v>
+      </c>
+      <c r="D48" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E48" s="17">
+        <v>43.301377992514034</v>
       </c>
     </row>
   </sheetData>
@@ -6363,8 +6581,8 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7051,6 +7269,12 @@
       <c r="C44" s="1">
         <v>44264.572222222225</v>
       </c>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>26.687696033767292</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -7062,6 +7286,12 @@
       <c r="C45" s="1">
         <v>44271.552083333336</v>
       </c>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>33.110132631793611</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -7073,6 +7303,12 @@
       <c r="C46" s="1">
         <v>44278.509722222225</v>
       </c>
+      <c r="D46" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E46" s="2">
+        <v>32.776386252166091</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -7084,6 +7320,12 @@
       <c r="C47" s="1">
         <v>44285.513194444444</v>
       </c>
+      <c r="D47" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E47" s="2">
+        <v>35.532989672068346</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -7094,6 +7336,12 @@
       </c>
       <c r="C48" s="1">
         <v>44296.527777777781</v>
+      </c>
+      <c r="D48" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E48" s="2">
+        <v>37.921105967012551</v>
       </c>
     </row>
   </sheetData>
@@ -7107,7 +7355,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7794,6 +8042,12 @@
       <c r="C44" s="1">
         <v>44264.587500000001</v>
       </c>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>119.58842791217491</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -7805,6 +8059,12 @@
       <c r="C45" s="1">
         <v>44271.567361111112</v>
       </c>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>216.15829621581724</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -7816,6 +8076,12 @@
       <c r="C46" s="1">
         <v>44278.525000000001</v>
       </c>
+      <c r="D46" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E46" s="2">
+        <v>181.1559819065115</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -7827,6 +8093,12 @@
       <c r="C47" s="1">
         <v>44285.568749999999</v>
       </c>
+      <c r="D47" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E47" s="2">
+        <v>196.96858805293633</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -7837,6 +8109,12 @@
       </c>
       <c r="C48" s="1">
         <v>44296.540277777778</v>
+      </c>
+      <c r="D48" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E48" s="2">
+        <v>170.4388219774419</v>
       </c>
     </row>
   </sheetData>
@@ -7850,7 +8128,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8493,7 +8771,7 @@
         <v>44258</v>
       </c>
       <c r="E41" s="2">
-        <v>1394.2534747665227</v>
+        <v>1443.5993000000001</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -8523,7 +8801,12 @@
       <c r="C43" s="1">
         <v>44264.6</v>
       </c>
-      <c r="D43" s="4"/>
+      <c r="D43" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E43" s="2">
+        <v>524.83763253677762</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
@@ -8535,7 +8818,12 @@
       <c r="C44" s="1">
         <v>44271.579861111109</v>
       </c>
-      <c r="D44" s="4"/>
+      <c r="D44" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E44" s="2">
+        <v>582.34346134481882</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
@@ -8547,7 +8835,12 @@
       <c r="C45" s="1">
         <v>44278.53402777778</v>
       </c>
-      <c r="D45" s="4"/>
+      <c r="D45" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E45" s="2">
+        <v>637.2314101001607</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
@@ -8559,7 +8852,12 @@
       <c r="C46" s="1">
         <v>44285.538194444445</v>
       </c>
-      <c r="D46" s="4"/>
+      <c r="D46" s="4">
+        <v>44306</v>
+      </c>
+      <c r="E46" s="2">
+        <v>480.66986537760374</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
@@ -8570,6 +8868,12 @@
       </c>
       <c r="C47" s="1">
         <v>44296.552083333336</v>
+      </c>
+      <c r="D47" s="4">
+        <v>44307</v>
+      </c>
+      <c r="E47" s="2">
+        <v>368.46121641355046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>